<commit_message>
curated TC07 diagnosis canine - stat bar query & function, cohort addition
</commit_message>
<xml_diff>
--- a/InputFiles/TC07_Canine_Filter_Diagnosis-TCellLymphoma.xlsx
+++ b/InputFiles/TC07_Canine_Filter_Diagnosis-TCellLymphoma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6AADD0-45DB-4A71-981C-C64905729DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5C95F-92F6-41AF-A6FD-16BA03399558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -63,22 +63,6 @@
     <t>TC07_Canine_Filter_Diagnosis-TCellLymphoma_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (s:study)
-  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
-  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
-  MATCH (d:diagnosis)
-  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
-  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-    WHERE diag.disease_term IN ['T Cell Lymphoma'] 
-  OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-  OPTIONAL MATCH (samp:sample)-[*]-&gt;(c)
-  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
-  RETURN count(DISTINCT(f)) as number_of_files ,
-             count(DISTINCT(samp)) as number_of_sample ,
-             count(DISTINCT(c.case_id)) as number_of_cases ,
-             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE diag.disease_term IN ['T Cell Lymphoma']
 WITH DISTINCT samp AS samp, c, demo, diag
@@ -128,7 +112,24 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+ WHERE diag.disease_term IN ['T Cell Lymphoma'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
 </sst>
 </file>
@@ -501,19 +502,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -530,15 +531,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -547,15 +548,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -564,15 +565,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>